<commit_message>
ready  for a new round of simulations
</commit_message>
<xml_diff>
--- a/inputTEMPLATE b.xlsx
+++ b/inputTEMPLATE b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>height</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>uptakeP04</t>
+  </si>
+  <si>
+    <t>uptake?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -958,299 +967,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="G1">
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="H1">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="I1">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="J1">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="L1">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="N1">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="O1">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="P1">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="R1">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="S1">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="T1">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="U1">
-        <v>17</v>
-      </c>
-      <c r="V1">
-        <v>18</v>
-      </c>
-      <c r="W1">
-        <v>19</v>
-      </c>
-      <c r="X1">
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>20</v>
       </c>
-      <c r="Y1">
-        <v>21</v>
-      </c>
-      <c r="Z1">
-        <v>22</v>
-      </c>
-      <c r="AA1">
-        <v>23</v>
-      </c>
-      <c r="AB1">
-        <v>24</v>
-      </c>
-      <c r="AC1">
-        <v>25</v>
-      </c>
-      <c r="AD1">
-        <v>26</v>
-      </c>
-      <c r="AE1">
-        <v>27</v>
-      </c>
-      <c r="AF1">
-        <v>28</v>
-      </c>
-      <c r="AG1">
-        <v>29</v>
-      </c>
-      <c r="AH1">
-        <v>30</v>
-      </c>
-      <c r="AI1">
-        <v>31</v>
-      </c>
-      <c r="AJ1">
-        <v>32</v>
-      </c>
-      <c r="AK1">
-        <v>33</v>
-      </c>
-      <c r="AL1">
-        <v>34</v>
-      </c>
-      <c r="AM1">
-        <v>35</v>
-      </c>
-      <c r="AN1">
-        <v>36</v>
-      </c>
-      <c r="AO1">
-        <v>37</v>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ref="C2" si="0">A2*B2</f>
+        <v>400</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f t="shared" ref="D2" si="1">IF(A2=B2,"square","rect")</f>
+        <v>square</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2" si="2">A2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>0.3</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0.3</v>
+      </c>
+      <c r="R2">
+        <v>0.3</v>
+      </c>
+      <c r="S2">
+        <v>0.1</v>
+      </c>
+      <c r="T2">
+        <v>0.1</v>
+      </c>
+      <c r="U2">
+        <v>0.1</v>
+      </c>
+      <c r="V2">
+        <v>0.1</v>
+      </c>
+      <c r="W2">
+        <v>42</v>
+      </c>
+      <c r="X2">
+        <v>42</v>
+      </c>
+      <c r="Y2">
+        <v>42</v>
+      </c>
+      <c r="Z2">
+        <v>42</v>
+      </c>
+      <c r="AA2">
+        <v>0.04</v>
+      </c>
+      <c r="AB2">
+        <v>0.04</v>
+      </c>
+      <c r="AC2">
+        <v>0.04</v>
+      </c>
+      <c r="AD2">
+        <v>0.04</v>
+      </c>
+      <c r="AE2">
+        <v>0.05</v>
+      </c>
+      <c r="AF2">
+        <v>0.05</v>
+      </c>
+      <c r="AG2">
+        <v>0.05</v>
+      </c>
+      <c r="AH2">
+        <v>0.05</v>
+      </c>
+      <c r="AI2">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ2">
+        <v>1E-3</v>
+      </c>
+      <c r="AK2">
+        <v>1E-3</v>
+      </c>
+      <c r="AL2">
+        <v>1E-3</v>
+      </c>
+      <c r="AM2">
+        <v>1E-3</v>
+      </c>
+      <c r="AN2">
+        <v>1E-3</v>
+      </c>
+      <c r="AO2">
+        <v>1E-3</v>
+      </c>
+      <c r="AP2">
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V2" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2" t="s">
-        <v>23</v>
-      </c>
-      <c r="X2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN2" t="s">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>40</v>
       </c>
-      <c r="AO2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>20</v>
-      </c>
       <c r="B3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3" si="0">A3*B3</f>
-        <v>400</v>
+        <f t="shared" ref="C3" si="3">A3*B3</f>
+        <v>1600</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3" si="1">IF(A3=B3,"square","rect")</f>
+        <f t="shared" ref="D3" si="4">IF(A3=B3,"square","rect")</f>
         <v>square</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3" si="2">A3/B3</f>
+        <f t="shared" ref="E3" si="5">A3/B3</f>
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>10</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>4</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
       <c r="K3">
         <v>2</v>
       </c>
@@ -1261,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>0.3</v>
@@ -1273,7 +1303,7 @@
         <v>0.3</v>
       </c>
       <c r="R3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="S3">
         <v>0.1</v>
@@ -1285,7 +1315,7 @@
         <v>0.1</v>
       </c>
       <c r="V3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="W3">
         <v>42</v>
@@ -1297,7 +1327,7 @@
         <v>42</v>
       </c>
       <c r="Z3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AA3">
         <v>0.04</v>
@@ -1309,7 +1339,7 @@
         <v>0.04</v>
       </c>
       <c r="AD3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AE3">
         <v>0.05</v>
@@ -1321,7 +1351,7 @@
         <v>0.05</v>
       </c>
       <c r="AH3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AI3">
         <v>1E-3</v>
@@ -1343,6 +1373,533 @@
       </c>
       <c r="AO3">
         <v>1E-3</v>
+      </c>
+      <c r="AP3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C6" si="6">A4*B4</f>
+        <v>10000</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" ref="D4:D6" si="7">IF(A4=B4,"square","rect")</f>
+        <v>square</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E6" si="8">A4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0.3</v>
+      </c>
+      <c r="P4">
+        <v>0.3</v>
+      </c>
+      <c r="Q4">
+        <v>0.3</v>
+      </c>
+      <c r="R4">
+        <v>0.3</v>
+      </c>
+      <c r="S4">
+        <v>0.1</v>
+      </c>
+      <c r="T4">
+        <v>0.1</v>
+      </c>
+      <c r="U4">
+        <v>0.1</v>
+      </c>
+      <c r="V4">
+        <v>0.1</v>
+      </c>
+      <c r="W4">
+        <v>42</v>
+      </c>
+      <c r="X4">
+        <v>42</v>
+      </c>
+      <c r="Y4">
+        <v>42</v>
+      </c>
+      <c r="Z4">
+        <v>42</v>
+      </c>
+      <c r="AA4">
+        <v>0.04</v>
+      </c>
+      <c r="AB4">
+        <v>0.04</v>
+      </c>
+      <c r="AC4">
+        <v>0.04</v>
+      </c>
+      <c r="AD4">
+        <v>0.04</v>
+      </c>
+      <c r="AE4">
+        <v>0.05</v>
+      </c>
+      <c r="AF4">
+        <v>0.05</v>
+      </c>
+      <c r="AG4">
+        <v>0.05</v>
+      </c>
+      <c r="AH4">
+        <v>0.05</v>
+      </c>
+      <c r="AI4">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ4">
+        <v>1E-3</v>
+      </c>
+      <c r="AK4">
+        <v>1E-3</v>
+      </c>
+      <c r="AL4">
+        <v>1E-3</v>
+      </c>
+      <c r="AM4">
+        <v>1E-3</v>
+      </c>
+      <c r="AN4">
+        <v>1E-3</v>
+      </c>
+      <c r="AO4">
+        <v>1E-3</v>
+      </c>
+      <c r="AP4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>square</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>0.3</v>
+      </c>
+      <c r="P5">
+        <v>0.3</v>
+      </c>
+      <c r="Q5">
+        <v>0.3</v>
+      </c>
+      <c r="R5">
+        <v>0.3</v>
+      </c>
+      <c r="S5">
+        <v>0.1</v>
+      </c>
+      <c r="T5">
+        <v>0.1</v>
+      </c>
+      <c r="U5">
+        <v>0.1</v>
+      </c>
+      <c r="V5">
+        <v>0.1</v>
+      </c>
+      <c r="W5">
+        <v>42</v>
+      </c>
+      <c r="X5">
+        <v>42</v>
+      </c>
+      <c r="Y5">
+        <v>42</v>
+      </c>
+      <c r="Z5">
+        <v>42</v>
+      </c>
+      <c r="AA5">
+        <v>0.04</v>
+      </c>
+      <c r="AB5">
+        <v>0.04</v>
+      </c>
+      <c r="AC5">
+        <v>0.04</v>
+      </c>
+      <c r="AD5">
+        <v>0.04</v>
+      </c>
+      <c r="AE5">
+        <v>0.05</v>
+      </c>
+      <c r="AF5">
+        <v>0.05</v>
+      </c>
+      <c r="AG5">
+        <v>0.05</v>
+      </c>
+      <c r="AH5">
+        <v>0.05</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="6"/>
+        <v>1600</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>square</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0.3</v>
+      </c>
+      <c r="P6">
+        <v>0.3</v>
+      </c>
+      <c r="Q6">
+        <v>0.3</v>
+      </c>
+      <c r="R6">
+        <v>0.3</v>
+      </c>
+      <c r="S6">
+        <v>0.1</v>
+      </c>
+      <c r="T6">
+        <v>0.1</v>
+      </c>
+      <c r="U6">
+        <v>0.1</v>
+      </c>
+      <c r="V6">
+        <v>0.1</v>
+      </c>
+      <c r="W6">
+        <v>42</v>
+      </c>
+      <c r="X6">
+        <v>42</v>
+      </c>
+      <c r="Y6">
+        <v>42</v>
+      </c>
+      <c r="Z6">
+        <v>42</v>
+      </c>
+      <c r="AA6">
+        <v>0.04</v>
+      </c>
+      <c r="AB6">
+        <v>0.04</v>
+      </c>
+      <c r="AC6">
+        <v>0.04</v>
+      </c>
+      <c r="AD6">
+        <v>0.04</v>
+      </c>
+      <c r="AE6">
+        <v>0.05</v>
+      </c>
+      <c r="AF6">
+        <v>0.05</v>
+      </c>
+      <c r="AG6">
+        <v>0.05</v>
+      </c>
+      <c r="AH6">
+        <v>0.05</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7" si="9">A7*B7</f>
+        <v>10000</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" ref="D7" si="10">IF(A7=B7,"square","rect")</f>
+        <v>square</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7" si="11">A7/B7</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>0.3</v>
+      </c>
+      <c r="P7">
+        <v>0.3</v>
+      </c>
+      <c r="Q7">
+        <v>0.3</v>
+      </c>
+      <c r="R7">
+        <v>0.3</v>
+      </c>
+      <c r="S7">
+        <v>0.1</v>
+      </c>
+      <c r="T7">
+        <v>0.1</v>
+      </c>
+      <c r="U7">
+        <v>0.1</v>
+      </c>
+      <c r="V7">
+        <v>0.1</v>
+      </c>
+      <c r="W7">
+        <v>42</v>
+      </c>
+      <c r="X7">
+        <v>42</v>
+      </c>
+      <c r="Y7">
+        <v>42</v>
+      </c>
+      <c r="Z7">
+        <v>42</v>
+      </c>
+      <c r="AA7">
+        <v>0.04</v>
+      </c>
+      <c r="AB7">
+        <v>0.04</v>
+      </c>
+      <c r="AC7">
+        <v>0.04</v>
+      </c>
+      <c r="AD7">
+        <v>0.04</v>
+      </c>
+      <c r="AE7">
+        <v>0.05</v>
+      </c>
+      <c r="AF7">
+        <v>0.05</v>
+      </c>
+      <c r="AG7">
+        <v>0.05</v>
+      </c>
+      <c r="AH7">
+        <v>0.05</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some simulation results with new LIST structure
</commit_message>
<xml_diff>
--- a/inputTEMPLATE b.xlsx
+++ b/inputTEMPLATE b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="210" windowWidth="28380" windowHeight="13230"/>
+    <workbookView xWindow="360" yWindow="210" windowWidth="19440" windowHeight="13230"/>
   </bookViews>
   <sheets>
     <sheet name="input06" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>height</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>TOTALN</t>
+  </si>
+  <si>
+    <t>TOTALP</t>
   </si>
 </sst>
 </file>
@@ -622,9 +628,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -967,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP7"/>
+  <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -982,13 +989,14 @@
     <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,107 +1024,113 @@
       <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1147,15 +1161,15 @@
       <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="2">
         <v>4</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
       <c r="M2">
         <v>2</v>
       </c>
@@ -1163,10 +1177,10 @@
         <v>2</v>
       </c>
       <c r="O2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q2">
         <v>0.3</v>
@@ -1175,10 +1189,10 @@
         <v>0.3</v>
       </c>
       <c r="S2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U2">
         <v>0.1</v>
@@ -1187,10 +1201,10 @@
         <v>0.1</v>
       </c>
       <c r="W2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y2">
         <v>42</v>
@@ -1199,10 +1213,10 @@
         <v>42</v>
       </c>
       <c r="AA2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC2">
         <v>0.04</v>
@@ -1211,10 +1225,10 @@
         <v>0.04</v>
       </c>
       <c r="AE2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG2">
         <v>0.05</v>
@@ -1223,10 +1237,10 @@
         <v>0.05</v>
       </c>
       <c r="AI2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AJ2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AK2">
         <v>1E-3</v>
@@ -1246,8 +1260,14 @@
       <c r="AP2">
         <v>1E-3</v>
       </c>
+      <c r="AQ2">
+        <v>1E-3</v>
+      </c>
+      <c r="AR2">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -1278,15 +1298,15 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="2">
         <v>4</v>
       </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
       <c r="M3">
         <v>2</v>
       </c>
@@ -1294,10 +1314,10 @@
         <v>2</v>
       </c>
       <c r="O3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q3">
         <v>0.3</v>
@@ -1306,10 +1326,10 @@
         <v>0.3</v>
       </c>
       <c r="S3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U3">
         <v>0.1</v>
@@ -1318,10 +1338,10 @@
         <v>0.1</v>
       </c>
       <c r="W3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y3">
         <v>42</v>
@@ -1330,10 +1350,10 @@
         <v>42</v>
       </c>
       <c r="AA3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC3">
         <v>0.04</v>
@@ -1342,10 +1362,10 @@
         <v>0.04</v>
       </c>
       <c r="AE3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG3">
         <v>0.05</v>
@@ -1354,10 +1374,10 @@
         <v>0.05</v>
       </c>
       <c r="AI3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AJ3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AK3">
         <v>1E-3</v>
@@ -1377,8 +1397,14 @@
       <c r="AP3">
         <v>1E-3</v>
       </c>
+      <c r="AQ3">
+        <v>1E-3</v>
+      </c>
+      <c r="AR3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1409,15 +1435,15 @@
       <c r="I4">
         <v>10</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="2">
         <v>4</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
       <c r="M4">
         <v>2</v>
       </c>
@@ -1425,10 +1451,10 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q4">
         <v>0.3</v>
@@ -1437,10 +1463,10 @@
         <v>0.3</v>
       </c>
       <c r="S4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U4">
         <v>0.1</v>
@@ -1449,10 +1475,10 @@
         <v>0.1</v>
       </c>
       <c r="W4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y4">
         <v>42</v>
@@ -1461,10 +1487,10 @@
         <v>42</v>
       </c>
       <c r="AA4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC4">
         <v>0.04</v>
@@ -1473,10 +1499,10 @@
         <v>0.04</v>
       </c>
       <c r="AE4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG4">
         <v>0.05</v>
@@ -1485,10 +1511,10 @@
         <v>0.05</v>
       </c>
       <c r="AI4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AJ4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AK4">
         <v>1E-3</v>
@@ -1508,8 +1534,14 @@
       <c r="AP4">
         <v>1E-3</v>
       </c>
+      <c r="AQ4">
+        <v>1E-3</v>
+      </c>
+      <c r="AR4">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1540,15 +1572,15 @@
       <c r="I5">
         <v>10</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="2">
         <v>4</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
       <c r="M5">
         <v>2</v>
       </c>
@@ -1556,10 +1588,10 @@
         <v>2</v>
       </c>
       <c r="O5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q5">
         <v>0.3</v>
@@ -1568,10 +1600,10 @@
         <v>0.3</v>
       </c>
       <c r="S5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U5">
         <v>0.1</v>
@@ -1580,10 +1612,10 @@
         <v>0.1</v>
       </c>
       <c r="W5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y5">
         <v>42</v>
@@ -1592,10 +1624,10 @@
         <v>42</v>
       </c>
       <c r="AA5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC5">
         <v>0.04</v>
@@ -1604,10 +1636,10 @@
         <v>0.04</v>
       </c>
       <c r="AE5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG5">
         <v>0.05</v>
@@ -1616,10 +1648,10 @@
         <v>0.05</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK5">
         <v>0</v>
@@ -1639,8 +1671,14 @@
       <c r="AP5">
         <v>0</v>
       </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1671,15 +1709,15 @@
       <c r="I6">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="2">
         <v>4</v>
       </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
       <c r="M6">
         <v>2</v>
       </c>
@@ -1687,10 +1725,10 @@
         <v>2</v>
       </c>
       <c r="O6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q6">
         <v>0.3</v>
@@ -1699,10 +1737,10 @@
         <v>0.3</v>
       </c>
       <c r="S6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U6">
         <v>0.1</v>
@@ -1711,10 +1749,10 @@
         <v>0.1</v>
       </c>
       <c r="W6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y6">
         <v>42</v>
@@ -1723,10 +1761,10 @@
         <v>42</v>
       </c>
       <c r="AA6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC6">
         <v>0.04</v>
@@ -1735,10 +1773,10 @@
         <v>0.04</v>
       </c>
       <c r="AE6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG6">
         <v>0.05</v>
@@ -1747,10 +1785,10 @@
         <v>0.05</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK6">
         <v>0</v>
@@ -1770,8 +1808,14 @@
       <c r="AP6">
         <v>0</v>
       </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -1802,15 +1846,15 @@
       <c r="I7">
         <v>10</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="2">
         <v>4</v>
       </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
       <c r="M7">
         <v>2</v>
       </c>
@@ -1818,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="O7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q7">
         <v>0.3</v>
@@ -1830,10 +1874,10 @@
         <v>0.3</v>
       </c>
       <c r="S7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="T7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="U7">
         <v>0.1</v>
@@ -1842,10 +1886,10 @@
         <v>0.1</v>
       </c>
       <c r="W7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="X7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Y7">
         <v>42</v>
@@ -1854,10 +1898,10 @@
         <v>42</v>
       </c>
       <c r="AA7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AB7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AC7">
         <v>0.04</v>
@@ -1866,10 +1910,10 @@
         <v>0.04</v>
       </c>
       <c r="AE7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AF7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AG7">
         <v>0.05</v>
@@ -1878,10 +1922,10 @@
         <v>0.05</v>
       </c>
       <c r="AI7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK7">
         <v>0</v>
@@ -1899,6 +1943,12 @@
         <v>0</v>
       </c>
       <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
loss is now a part of input.csv - compatible w/ GROW(), INPUT2(), and SPECIES2()
</commit_message>
<xml_diff>
--- a/inputTEMPLATE b.xlsx
+++ b/inputTEMPLATE b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>height</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>TOTALP</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -974,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -990,13 +993,14 @@
     <col min="6" max="7" width="9.140625" style="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1031,106 +1035,109 @@
         <v>46</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1168,11 +1175,11 @@
         <v>0.5</v>
       </c>
       <c r="L2" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M2" s="2">
         <v>4</v>
       </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
       <c r="N2">
         <v>2</v>
       </c>
@@ -1183,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="Q2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R2">
         <v>0.3</v>
@@ -1195,7 +1202,7 @@
         <v>0.3</v>
       </c>
       <c r="U2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V2">
         <v>0.1</v>
@@ -1207,7 +1214,7 @@
         <v>0.1</v>
       </c>
       <c r="Y2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z2">
         <v>42</v>
@@ -1219,7 +1226,7 @@
         <v>42</v>
       </c>
       <c r="AC2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD2">
         <v>0.04</v>
@@ -1231,7 +1238,7 @@
         <v>0.04</v>
       </c>
       <c r="AG2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH2">
         <v>0.05</v>
@@ -1243,7 +1250,7 @@
         <v>0.05</v>
       </c>
       <c r="AK2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AL2">
         <v>1E-3</v>
@@ -1266,8 +1273,11 @@
       <c r="AR2">
         <v>1E-3</v>
       </c>
+      <c r="AS2">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -1305,11 +1315,11 @@
         <v>0.5</v>
       </c>
       <c r="L3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="2">
         <v>4</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
       <c r="N3">
         <v>2</v>
       </c>
@@ -1320,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="Q3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R3">
         <v>0.3</v>
@@ -1332,7 +1342,7 @@
         <v>0.3</v>
       </c>
       <c r="U3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V3">
         <v>0.1</v>
@@ -1344,7 +1354,7 @@
         <v>0.1</v>
       </c>
       <c r="Y3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z3">
         <v>42</v>
@@ -1356,7 +1366,7 @@
         <v>42</v>
       </c>
       <c r="AC3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD3">
         <v>0.04</v>
@@ -1368,7 +1378,7 @@
         <v>0.04</v>
       </c>
       <c r="AG3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH3">
         <v>0.05</v>
@@ -1380,7 +1390,7 @@
         <v>0.05</v>
       </c>
       <c r="AK3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AL3">
         <v>1E-3</v>
@@ -1403,8 +1413,11 @@
       <c r="AR3">
         <v>1E-3</v>
       </c>
+      <c r="AS3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1442,11 +1455,11 @@
         <v>0.5</v>
       </c>
       <c r="L4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="2">
         <v>4</v>
       </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
       <c r="N4">
         <v>2</v>
       </c>
@@ -1457,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R4">
         <v>0.3</v>
@@ -1469,7 +1482,7 @@
         <v>0.3</v>
       </c>
       <c r="U4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V4">
         <v>0.1</v>
@@ -1481,7 +1494,7 @@
         <v>0.1</v>
       </c>
       <c r="Y4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z4">
         <v>42</v>
@@ -1493,7 +1506,7 @@
         <v>42</v>
       </c>
       <c r="AC4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD4">
         <v>0.04</v>
@@ -1505,7 +1518,7 @@
         <v>0.04</v>
       </c>
       <c r="AG4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH4">
         <v>0.05</v>
@@ -1517,7 +1530,7 @@
         <v>0.05</v>
       </c>
       <c r="AK4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AL4">
         <v>1E-3</v>
@@ -1540,8 +1553,11 @@
       <c r="AR4">
         <v>1E-3</v>
       </c>
+      <c r="AS4">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1579,11 +1595,11 @@
         <v>0.5</v>
       </c>
       <c r="L5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="2">
         <v>4</v>
       </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
       <c r="N5">
         <v>2</v>
       </c>
@@ -1594,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="Q5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R5">
         <v>0.3</v>
@@ -1606,7 +1622,7 @@
         <v>0.3</v>
       </c>
       <c r="U5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V5">
         <v>0.1</v>
@@ -1618,7 +1634,7 @@
         <v>0.1</v>
       </c>
       <c r="Y5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z5">
         <v>42</v>
@@ -1630,7 +1646,7 @@
         <v>42</v>
       </c>
       <c r="AC5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD5">
         <v>0.04</v>
@@ -1642,7 +1658,7 @@
         <v>0.04</v>
       </c>
       <c r="AG5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH5">
         <v>0.05</v>
@@ -1654,7 +1670,7 @@
         <v>0.05</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AL5">
         <v>0</v>
@@ -1677,8 +1693,11 @@
       <c r="AR5">
         <v>0</v>
       </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1716,11 +1735,11 @@
         <v>0.5</v>
       </c>
       <c r="L6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M6" s="2">
         <v>4</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
       <c r="N6">
         <v>2</v>
       </c>
@@ -1731,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="Q6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R6">
         <v>0.3</v>
@@ -1743,7 +1762,7 @@
         <v>0.3</v>
       </c>
       <c r="U6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V6">
         <v>0.1</v>
@@ -1755,7 +1774,7 @@
         <v>0.1</v>
       </c>
       <c r="Y6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z6">
         <v>42</v>
@@ -1767,7 +1786,7 @@
         <v>42</v>
       </c>
       <c r="AC6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD6">
         <v>0.04</v>
@@ -1779,7 +1798,7 @@
         <v>0.04</v>
       </c>
       <c r="AG6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH6">
         <v>0.05</v>
@@ -1791,7 +1810,7 @@
         <v>0.05</v>
       </c>
       <c r="AK6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AL6">
         <v>0</v>
@@ -1814,8 +1833,11 @@
       <c r="AR6">
         <v>0</v>
       </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -1853,11 +1875,11 @@
         <v>0.5</v>
       </c>
       <c r="L7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="M7" s="2">
         <v>4</v>
       </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
       <c r="N7">
         <v>2</v>
       </c>
@@ -1868,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="Q7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R7">
         <v>0.3</v>
@@ -1880,7 +1902,7 @@
         <v>0.3</v>
       </c>
       <c r="U7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="V7">
         <v>0.1</v>
@@ -1892,7 +1914,7 @@
         <v>0.1</v>
       </c>
       <c r="Y7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="Z7">
         <v>42</v>
@@ -1904,7 +1926,7 @@
         <v>42</v>
       </c>
       <c r="AC7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AD7">
         <v>0.04</v>
@@ -1916,7 +1938,7 @@
         <v>0.04</v>
       </c>
       <c r="AG7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AH7">
         <v>0.05</v>
@@ -1928,7 +1950,7 @@
         <v>0.05</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AL7">
         <v>0</v>
@@ -1949,6 +1971,9 @@
         <v>0</v>
       </c>
       <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
model needs to include both initial # of cells occupied and total initial biomass
</commit_message>
<xml_diff>
--- a/inputTEMPLATE b.xlsx
+++ b/inputTEMPLATE b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>height</t>
   </si>
@@ -31,18 +31,6 @@
     <t>numbspecies</t>
   </si>
   <si>
-    <t>initial01</t>
-  </si>
-  <si>
-    <t>initial02</t>
-  </si>
-  <si>
-    <t>initial03</t>
-  </si>
-  <si>
-    <t>initial04</t>
-  </si>
-  <si>
     <t>maxrgr01</t>
   </si>
   <si>
@@ -158,6 +146,30 @@
   </si>
   <si>
     <t>loss</t>
+  </si>
+  <si>
+    <t>initial01cells</t>
+  </si>
+  <si>
+    <t>initial02cells</t>
+  </si>
+  <si>
+    <t>initial03cells</t>
+  </si>
+  <si>
+    <t>initial04cells</t>
+  </si>
+  <si>
+    <t>initial01totmass</t>
+  </si>
+  <si>
+    <t>initial02totmass</t>
+  </si>
+  <si>
+    <t>initial03totmass</t>
+  </si>
+  <si>
+    <t>initial04totmass</t>
   </si>
 </sst>
 </file>
@@ -977,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -995,12 +1007,13 @@
     <col min="10" max="11" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="2" customWidth="1"/>
     <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1008,19 +1021,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -1029,115 +1042,127 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Y1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AI1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AP1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AS1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AT1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AU1" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1157,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H2">
         <v>100</v>
@@ -1193,76 +1218,76 @@
         <v>2</v>
       </c>
       <c r="R2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AM2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AN2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AO2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AP2">
         <v>1E-3</v>
@@ -1276,8 +1301,20 @@
       <c r="AS2">
         <v>1E-3</v>
       </c>
+      <c r="AT2">
+        <v>1E-3</v>
+      </c>
+      <c r="AU2">
+        <v>1E-3</v>
+      </c>
+      <c r="AV2">
+        <v>1E-3</v>
+      </c>
+      <c r="AW2">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -1297,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -1333,76 +1370,76 @@
         <v>2</v>
       </c>
       <c r="R3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AM3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AN3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AO3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AP3">
         <v>1E-3</v>
@@ -1416,8 +1453,20 @@
       <c r="AS3">
         <v>1E-3</v>
       </c>
+      <c r="AT3">
+        <v>1E-3</v>
+      </c>
+      <c r="AU3">
+        <v>1E-3</v>
+      </c>
+      <c r="AV3">
+        <v>1E-3</v>
+      </c>
+      <c r="AW3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1437,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -1473,76 +1522,76 @@
         <v>2</v>
       </c>
       <c r="R4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AM4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AN4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AO4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AP4">
         <v>1E-3</v>
@@ -1556,8 +1605,20 @@
       <c r="AS4">
         <v>1E-3</v>
       </c>
+      <c r="AT4">
+        <v>1E-3</v>
+      </c>
+      <c r="AU4">
+        <v>1E-3</v>
+      </c>
+      <c r="AV4">
+        <v>1E-3</v>
+      </c>
+      <c r="AW4">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1577,10 +1638,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>100</v>
@@ -1613,76 +1674,76 @@
         <v>2</v>
       </c>
       <c r="R5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AO5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AP5">
         <v>0</v>
@@ -1696,8 +1757,20 @@
       <c r="AS5">
         <v>0</v>
       </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1717,10 +1790,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>100</v>
@@ -1753,76 +1826,76 @@
         <v>2</v>
       </c>
       <c r="R6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AM6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AN6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AO6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AP6">
         <v>0</v>
@@ -1836,8 +1909,20 @@
       <c r="AS6">
         <v>0</v>
       </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -1857,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H7">
         <v>100</v>
@@ -1893,76 +1978,76 @@
         <v>2</v>
       </c>
       <c r="R7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="S7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="T7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="V7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="W7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Y7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="Z7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AA7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AB7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AC7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AD7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AE7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AF7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AG7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AH7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AI7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AJ7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AK7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AL7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AN7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AO7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AP7">
         <v>0</v>
@@ -1974,6 +2059,18 @@
         <v>0</v>
       </c>
       <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
amounttomove and thresholdtomove are now a part of the input.csv system
</commit_message>
<xml_diff>
--- a/inputTEMPLATE b.xlsx
+++ b/inputTEMPLATE b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>height</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>initial04totmass</t>
+  </si>
+  <si>
+    <t>thresholdtomove</t>
+  </si>
+  <si>
+    <t>amounttomove</t>
   </si>
 </sst>
 </file>
@@ -989,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW7"/>
+  <dimension ref="A1:AY7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="M2" sqref="M2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1005,15 +1011,15 @@
     <col min="6" max="7" width="9.140625" style="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,118 +1057,124 @@
         <v>43</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>47</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>48</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>49</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>50</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>51</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>5</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>6</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>25</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>31</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>33</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>34</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1203,14 +1215,14 @@
         <v>0.05</v>
       </c>
       <c r="M2" s="2">
+        <v>30</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O2" s="2">
         <v>4</v>
       </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
       <c r="P2">
         <v>2</v>
       </c>
@@ -1230,10 +1242,10 @@
         <v>2</v>
       </c>
       <c r="V2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X2">
         <v>0.3</v>
@@ -1242,10 +1254,10 @@
         <v>0.3</v>
       </c>
       <c r="Z2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB2">
         <v>0.1</v>
@@ -1254,10 +1266,10 @@
         <v>0.1</v>
       </c>
       <c r="AD2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE2">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF2">
         <v>42</v>
@@ -1266,10 +1278,10 @@
         <v>42</v>
       </c>
       <c r="AH2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI2">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ2">
         <v>0.04</v>
@@ -1278,10 +1290,10 @@
         <v>0.04</v>
       </c>
       <c r="AL2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN2">
         <v>0.05</v>
@@ -1290,10 +1302,10 @@
         <v>0.05</v>
       </c>
       <c r="AP2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AQ2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AR2">
         <v>1E-3</v>
@@ -1313,8 +1325,14 @@
       <c r="AW2">
         <v>1E-3</v>
       </c>
+      <c r="AX2">
+        <v>1E-3</v>
+      </c>
+      <c r="AY2">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -1355,14 +1373,14 @@
         <v>0.05</v>
       </c>
       <c r="M3" s="2">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O3" s="2">
         <v>4</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
       <c r="P3">
         <v>2</v>
       </c>
@@ -1382,10 +1400,10 @@
         <v>2</v>
       </c>
       <c r="V3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W3">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X3">
         <v>0.3</v>
@@ -1394,10 +1412,10 @@
         <v>0.3</v>
       </c>
       <c r="Z3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB3">
         <v>0.1</v>
@@ -1406,10 +1424,10 @@
         <v>0.1</v>
       </c>
       <c r="AD3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE3">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF3">
         <v>42</v>
@@ -1418,10 +1436,10 @@
         <v>42</v>
       </c>
       <c r="AH3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI3">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ3">
         <v>0.04</v>
@@ -1430,10 +1448,10 @@
         <v>0.04</v>
       </c>
       <c r="AL3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN3">
         <v>0.05</v>
@@ -1442,10 +1460,10 @@
         <v>0.05</v>
       </c>
       <c r="AP3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AQ3">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AR3">
         <v>1E-3</v>
@@ -1465,8 +1483,14 @@
       <c r="AW3">
         <v>1E-3</v>
       </c>
+      <c r="AX3">
+        <v>1E-3</v>
+      </c>
+      <c r="AY3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1507,14 +1531,14 @@
         <v>0.05</v>
       </c>
       <c r="M4" s="2">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O4" s="2">
         <v>4</v>
       </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
       <c r="P4">
         <v>2</v>
       </c>
@@ -1534,10 +1558,10 @@
         <v>2</v>
       </c>
       <c r="V4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W4">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X4">
         <v>0.3</v>
@@ -1546,10 +1570,10 @@
         <v>0.3</v>
       </c>
       <c r="Z4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB4">
         <v>0.1</v>
@@ -1558,10 +1582,10 @@
         <v>0.1</v>
       </c>
       <c r="AD4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE4">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF4">
         <v>42</v>
@@ -1570,10 +1594,10 @@
         <v>42</v>
       </c>
       <c r="AH4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI4">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ4">
         <v>0.04</v>
@@ -1582,10 +1606,10 @@
         <v>0.04</v>
       </c>
       <c r="AL4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN4">
         <v>0.05</v>
@@ -1594,10 +1618,10 @@
         <v>0.05</v>
       </c>
       <c r="AP4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AQ4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AR4">
         <v>1E-3</v>
@@ -1617,8 +1641,14 @@
       <c r="AW4">
         <v>1E-3</v>
       </c>
+      <c r="AX4">
+        <v>1E-3</v>
+      </c>
+      <c r="AY4">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1659,14 +1689,14 @@
         <v>0.05</v>
       </c>
       <c r="M5" s="2">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O5" s="2">
         <v>4</v>
       </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
       <c r="P5">
         <v>2</v>
       </c>
@@ -1686,10 +1716,10 @@
         <v>2</v>
       </c>
       <c r="V5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X5">
         <v>0.3</v>
@@ -1698,10 +1728,10 @@
         <v>0.3</v>
       </c>
       <c r="Z5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB5">
         <v>0.1</v>
@@ -1710,10 +1740,10 @@
         <v>0.1</v>
       </c>
       <c r="AD5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE5">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF5">
         <v>42</v>
@@ -1722,10 +1752,10 @@
         <v>42</v>
       </c>
       <c r="AH5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI5">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ5">
         <v>0.04</v>
@@ -1734,10 +1764,10 @@
         <v>0.04</v>
       </c>
       <c r="AL5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN5">
         <v>0.05</v>
@@ -1746,10 +1776,10 @@
         <v>0.05</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AR5">
         <v>0</v>
@@ -1769,8 +1799,14 @@
       <c r="AW5">
         <v>0</v>
       </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1811,14 +1847,14 @@
         <v>0.05</v>
       </c>
       <c r="M6" s="2">
+        <v>30</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O6" s="2">
         <v>4</v>
       </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
       <c r="P6">
         <v>2</v>
       </c>
@@ -1838,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="V6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X6">
         <v>0.3</v>
@@ -1850,10 +1886,10 @@
         <v>0.3</v>
       </c>
       <c r="Z6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB6">
         <v>0.1</v>
@@ -1862,10 +1898,10 @@
         <v>0.1</v>
       </c>
       <c r="AD6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE6">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF6">
         <v>42</v>
@@ -1874,10 +1910,10 @@
         <v>42</v>
       </c>
       <c r="AH6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI6">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ6">
         <v>0.04</v>
@@ -1886,10 +1922,10 @@
         <v>0.04</v>
       </c>
       <c r="AL6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN6">
         <v>0.05</v>
@@ -1898,10 +1934,10 @@
         <v>0.05</v>
       </c>
       <c r="AP6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AR6">
         <v>0</v>
@@ -1921,8 +1957,14 @@
       <c r="AW6">
         <v>0</v>
       </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -1963,14 +2005,14 @@
         <v>0.05</v>
       </c>
       <c r="M7" s="2">
+        <v>30</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O7" s="2">
         <v>4</v>
       </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
       <c r="P7">
         <v>2</v>
       </c>
@@ -1990,10 +2032,10 @@
         <v>2</v>
       </c>
       <c r="V7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="W7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="X7">
         <v>0.3</v>
@@ -2002,10 +2044,10 @@
         <v>0.3</v>
       </c>
       <c r="Z7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AB7">
         <v>0.1</v>
@@ -2014,10 +2056,10 @@
         <v>0.1</v>
       </c>
       <c r="AD7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AE7">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="AF7">
         <v>42</v>
@@ -2026,10 +2068,10 @@
         <v>42</v>
       </c>
       <c r="AH7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AI7">
-        <v>0.04</v>
+        <v>42</v>
       </c>
       <c r="AJ7">
         <v>0.04</v>
@@ -2038,10 +2080,10 @@
         <v>0.04</v>
       </c>
       <c r="AL7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AM7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AN7">
         <v>0.05</v>
@@ -2050,10 +2092,10 @@
         <v>0.05</v>
       </c>
       <c r="AP7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AR7">
         <v>0</v>
@@ -2071,6 +2113,12 @@
         <v>0</v>
       </c>
       <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
         <v>0</v>
       </c>
     </row>

</xml_diff>